<commit_message>
# Please enter the commit message for your changes. Lines starting # with '#' will be ignored, and an empty message aborts the commit. # # On branch main # Your branch is up to date with 'origin/main'. # # Changes to be committed: #	new file:   .idea/SucessfulAlgoTrading.iml #	new file:   .idea/inspectionProfiles/profiles_settings.xml #	new file:   .idea/misc.xml #	new file:   .idea/modules.xml #	new file:   .idea/vcs.xml #	new file:   .idea/workspace.xml #	new file:   dhan/bin/Buy_options.ipynb #	modified:   dhan/bin/Options.xlsx #	modified:   dhan/bin/security_id_list.csv #	modified:   dhan/bin/step_1_get_required_security_ids.ipynb #	modified:   dhan/bin/underlying.xlsx #	new file:   dhan/bin/websocket.py #	modified:   dhan/configs/config.yaml
</commit_message>
<xml_diff>
--- a/dhan/bin/underlying.xlsx
+++ b/dhan/bin/underlying.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,19 +447,29 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>435823</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CRUDEOIL</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>13</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>NIFTY</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="4">
+      <c r="A4" t="n">
         <v>25</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>BANKNIFTY</t>
         </is>

</xml_diff>